<commit_message>
Projectile started,good on serv side
</commit_message>
<xml_diff>
--- a/data/Envoie_données.xlsx
+++ b/data/Envoie_données.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nobil\Unknown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nobil\Unknown\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78B7973-B4D4-4CA5-91F7-93EB73A1F893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501248C4-E3C6-40D4-B890-335B5D18F863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{B9327B43-8E89-4C75-A473-2C353B32A7CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>ID send</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>chunk/id/new_pos</t>
+  </si>
+  <si>
+    <t>projectile_create</t>
+  </si>
+  <si>
+    <t>projectile_die</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C48EE1-EBD0-4B79-91FA-27BBFC80C012}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -620,6 +626,22 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Can switch spell in weapon
</commit_message>
<xml_diff>
--- a/data/Envoie_données.xlsx
+++ b/data/Envoie_données.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nobil\Unknown\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137E3614-CCFB-416A-8423-D2E73E762277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A922F444-7BFD-4EF9-B2A0-33CDE8C5634D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{B9327B43-8E89-4C75-A473-2C353B32A7CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>ID send</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>id player / new_life</t>
+  </si>
+  <si>
+    <t>Switch spell_pos</t>
+  </si>
+  <si>
+    <t>(weapon/idx)(weapon/idx)</t>
   </si>
 </sst>
 </file>
@@ -506,13 +512,13 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="31.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="25.73046875" customWidth="1"/>
     <col min="8" max="8" width="28.19921875" customWidth="1"/>
   </cols>
@@ -620,6 +626,15 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
       <c r="F7">
         <v>5</v>
       </c>

</xml_diff>